<commit_message>
add gama var and run in linux server
</commit_message>
<xml_diff>
--- a/src/data/W/W_0.xlsx
+++ b/src/data/W/W_0.xlsx
@@ -470,13 +470,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1948938640805274</v>
+        <v>0.2507682433729189</v>
       </c>
       <c r="C2" t="n">
-        <v>140.0193435832487</v>
+        <v>139.9984142924607</v>
       </c>
       <c r="D2" t="n">
-        <v>26.58062490376419</v>
+        <v>26.60770010622114</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -490,13 +490,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.363893357295271</v>
+        <v>0.2381696006674072</v>
       </c>
       <c r="C3" t="n">
-        <v>149.967522862923</v>
+        <v>150.0154066158082</v>
       </c>
       <c r="D3" t="n">
-        <v>30.60471286643586</v>
+        <v>30.57983537447953</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -510,13 +510,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3364068093289763</v>
+        <v>0.5591187777121429</v>
       </c>
       <c r="C4" t="n">
-        <v>169.9855475208577</v>
+        <v>169.9935135404647</v>
       </c>
       <c r="D4" t="n">
-        <v>45.25149359395074</v>
+        <v>45.23821949040304</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -530,13 +530,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2395284232052413</v>
+        <v>0.2162014613825038</v>
       </c>
       <c r="C5" t="n">
-        <v>190.0232882172818</v>
+        <v>190.010250972039</v>
       </c>
       <c r="D5" t="n">
-        <v>59.84107199992053</v>
+        <v>59.8842385324773</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -550,13 +550,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3550373360066262</v>
+        <v>0.4345211289839501</v>
       </c>
       <c r="C6" t="n">
-        <v>199.9717744050359</v>
+        <v>199.9506357312878</v>
       </c>
       <c r="D6" t="n">
-        <v>101.0746942563768</v>
+        <v>101.0966366979837</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -570,13 +570,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4750498149127194</v>
+        <v>0.362585117781934</v>
       </c>
       <c r="C7" t="n">
-        <v>220.0233551335889</v>
+        <v>219.9635952686818</v>
       </c>
       <c r="D7" t="n">
-        <v>119.7449398989319</v>
+        <v>119.692488131674</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -590,13 +590,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9431419315519579</v>
+        <v>0.6720973592288922</v>
       </c>
       <c r="C8" t="n">
-        <v>230.0048538988419</v>
+        <v>229.9760519082197</v>
       </c>
       <c r="D8" t="n">
-        <v>159.6441971515846</v>
+        <v>159.6033326279629</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -610,19 +610,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.098504163991985</v>
+        <v>1.120178800818433</v>
       </c>
       <c r="C9" t="n">
-        <v>240.0120116905156</v>
+        <v>239.9592720341348</v>
       </c>
       <c r="D9" t="n">
-        <v>199.4913620708023</v>
+        <v>199.5140432874598</v>
       </c>
       <c r="E9" t="n">
-        <v>10.03624687242333</v>
+        <v>10.02459394719106</v>
       </c>
       <c r="F9" t="n">
-        <v>107.3688706829638</v>
+        <v>107.428872800964</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.138084660586991</v>
+        <v>0.9937320674031552</v>
       </c>
       <c r="C10" t="n">
-        <v>259.9979176184856</v>
+        <v>260.0090442692743</v>
       </c>
       <c r="D10" t="n">
-        <v>239.4201016881424</v>
+        <v>239.4739650880558</v>
       </c>
       <c r="E10" t="n">
-        <v>11.00732581543396</v>
+        <v>11.01128368342348</v>
       </c>
       <c r="F10" t="n">
-        <v>39.52185676710464</v>
+        <v>39.72116572418403</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.044782194245523</v>
+        <v>1.055731506605515</v>
       </c>
       <c r="C11" t="n">
-        <v>279.9968365512411</v>
+        <v>279.9618428123343</v>
       </c>
       <c r="D11" t="n">
-        <v>266.0988835103635</v>
+        <v>266.0068096765842</v>
       </c>
       <c r="E11" t="n">
-        <v>12.01555498103868</v>
+        <v>11.93321570346827</v>
       </c>
       <c r="F11" t="n">
-        <v>82.99180458513871</v>
+        <v>83.17479577808436</v>
       </c>
     </row>
     <row r="12">
@@ -670,19 +670,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6228553639509067</v>
+        <v>0.7433042895197757</v>
       </c>
       <c r="C12" t="n">
-        <v>289.9900485807837</v>
+        <v>290.029155460542</v>
       </c>
       <c r="D12" t="n">
-        <v>279.2908993548667</v>
+        <v>279.3085890012551</v>
       </c>
       <c r="E12" t="n">
-        <v>13.00890549744954</v>
+        <v>12.98284862508489</v>
       </c>
       <c r="F12" t="n">
-        <v>127.9596911222766</v>
+        <v>128.0326565291527</v>
       </c>
     </row>
     <row r="13">
@@ -690,19 +690,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.8858311937152421</v>
+        <v>0.8897395155988221</v>
       </c>
       <c r="C13" t="n">
-        <v>291.979555282688</v>
+        <v>292.02530816954</v>
       </c>
       <c r="D13" t="n">
-        <v>266.0244669796883</v>
+        <v>266.0875395603134</v>
       </c>
       <c r="E13" t="n">
-        <v>13.94332707924577</v>
+        <v>13.98355206655079</v>
       </c>
       <c r="F13" t="n">
-        <v>156.8868933558933</v>
+        <v>156.8073350724999</v>
       </c>
     </row>
     <row r="14">
@@ -710,19 +710,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.9195938986001979</v>
+        <v>0.700772150331292</v>
       </c>
       <c r="C14" t="n">
-        <v>280.0636679201732</v>
+        <v>279.9572568635565</v>
       </c>
       <c r="D14" t="n">
-        <v>248.7501612242011</v>
+        <v>248.7352580026164</v>
       </c>
       <c r="E14" t="n">
-        <v>15.00394830150621</v>
+        <v>14.98496965002514</v>
       </c>
       <c r="F14" t="n">
-        <v>145.9347003113454</v>
+        <v>145.7498599921738</v>
       </c>
     </row>
     <row r="15">
@@ -730,19 +730,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.8010617464089373</v>
+        <v>0.7840141341245218</v>
       </c>
       <c r="C15" t="n">
-        <v>259.9337368036694</v>
+        <v>259.929675378562</v>
       </c>
       <c r="D15" t="n">
-        <v>234.1132913152871</v>
+        <v>234.1179635629287</v>
       </c>
       <c r="E15" t="n">
-        <v>15.95840676743833</v>
+        <v>15.99151689977768</v>
       </c>
       <c r="F15" t="n">
-        <v>169.8911204502799</v>
+        <v>170.0047751077827</v>
       </c>
     </row>
     <row r="16">
@@ -750,19 +750,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.7124742988440381</v>
+        <v>0.9788096679358043</v>
       </c>
       <c r="C16" t="n">
-        <v>252.3793859703812</v>
+        <v>252.3987584964777</v>
       </c>
       <c r="D16" t="n">
-        <v>219.4356072237056</v>
+        <v>219.4662726748273</v>
       </c>
       <c r="E16" t="n">
-        <v>17.03282032259311</v>
+        <v>16.979276812169</v>
       </c>
       <c r="F16" t="n">
-        <v>165.5636727996647</v>
+        <v>165.7068221548472</v>
       </c>
     </row>
     <row r="17">
@@ -770,19 +770,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1.03977461850159</v>
+        <v>1.058961198360017</v>
       </c>
       <c r="C17" t="n">
-        <v>251.1940564316711</v>
+        <v>251.1828820852019</v>
       </c>
       <c r="D17" t="n">
-        <v>219.5000084855446</v>
+        <v>219.4818665510647</v>
       </c>
       <c r="E17" t="n">
-        <v>18.02462986660683</v>
+        <v>17.9896355840418</v>
       </c>
       <c r="F17" t="n">
-        <v>130.2249204935351</v>
+        <v>130.2515972013716</v>
       </c>
     </row>
     <row r="18">
@@ -790,16 +790,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1.262739267359442</v>
+        <v>1.073699590780893</v>
       </c>
       <c r="C18" t="n">
-        <v>248.0058777888713</v>
+        <v>247.9861182083281</v>
       </c>
       <c r="D18" t="n">
-        <v>218.1399170501199</v>
+        <v>218.1831791621452</v>
       </c>
       <c r="E18" t="n">
-        <v>19.00428320194971</v>
+        <v>19.01136481086589</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -810,16 +810,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.206118018367341</v>
+        <v>1.149208626085906</v>
       </c>
       <c r="C19" t="n">
-        <v>246.3723659476744</v>
+        <v>246.334776456127</v>
       </c>
       <c r="D19" t="n">
-        <v>214.1976945646265</v>
+        <v>214.1341865826534</v>
       </c>
       <c r="E19" t="n">
-        <v>20.00219538490347</v>
+        <v>19.99436379437963</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -830,16 +830,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.160209632405763</v>
+        <v>1.221161738781391</v>
       </c>
       <c r="C20" t="n">
-        <v>245.5586099593222</v>
+        <v>245.61328035039</v>
       </c>
       <c r="D20" t="n">
-        <v>212.869547511565</v>
+        <v>212.7907394884319</v>
       </c>
       <c r="E20" t="n">
-        <v>20.97094943102717</v>
+        <v>21.05292847795123</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -850,13 +850,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1.057773441520963</v>
+        <v>1.06616396739849</v>
       </c>
       <c r="C21" t="n">
-        <v>243.9516798335985</v>
+        <v>244.0086602325569</v>
       </c>
       <c r="D21" t="n">
-        <v>199.5535961177405</v>
+        <v>199.5298871748793</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -870,13 +870,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.6445835922979993</v>
+        <v>0.9490997908407564</v>
       </c>
       <c r="C22" t="n">
-        <v>239.928497288322</v>
+        <v>240.0228911109342</v>
       </c>
       <c r="D22" t="n">
-        <v>172.9415092326897</v>
+        <v>172.9531448331074</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -890,13 +890,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.6683539789117505</v>
+        <v>0.9401319404023937</v>
       </c>
       <c r="C23" t="n">
-        <v>219.9919711013017</v>
+        <v>220.0225668827591</v>
       </c>
       <c r="D23" t="n">
-        <v>106.4563664726016</v>
+        <v>106.4419472085371</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -910,13 +910,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.4445029566144274</v>
+        <v>0.3043630684718461</v>
       </c>
       <c r="C24" t="n">
-        <v>180.0293799750212</v>
+        <v>179.9890088783918</v>
       </c>
       <c r="D24" t="n">
-        <v>66.47170384962639</v>
+        <v>66.50901503715228</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -930,13 +930,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.3004776823209239</v>
+        <v>0.3976597549510634</v>
       </c>
       <c r="C25" t="n">
-        <v>159.9796528046684</v>
+        <v>159.9767571910015</v>
       </c>
       <c r="D25" t="n">
-        <v>39.89458682058181</v>
+        <v>39.92697972083772</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>

</xml_diff>